<commit_message>
Add OOPath runtime benchmarks
</commit_message>
<xml_diff>
--- a/drools-benchmarks/src/main/resources/kbase-creation/oopath-kbase-creation.xlsx
+++ b/drools-benchmarks/src/main/resources/kbase-creation/oopath-kbase-creation.xlsx
@@ -38,6 +38,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">A keyword of "Ruleset" means that this worksheet is a ruleset, and it has a name in the next cell across. In the following lines, we can have imports, or other ruleset directives if we need to ad them in future.
 </t>
@@ -48,6 +49,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Perhaps this is not needed - ruleset name can be XLS name, and imports are not really needed most of the time.</t>
         </r>
@@ -62,6 +64,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Look at me !! I tell you that I am the start of a rule table, and what parameters I require !
 </t>
@@ -72,6 +75,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">(and their types).
 The "RuleTable" keyword must appear on top of the first condition column.
@@ -89,6 +93,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Look at me !!
 </t>
@@ -99,6 +104,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">I tell you that I am a condition colmn. The next row down has the rule "template" and the row below that is a comment. After that, it is all rule data until an empty line !
 Note that if there is no data in a row, then this condition does not apply. 
@@ -123,7 +129,7 @@
     <t xml:space="preserve">Import</t>
   </si>
   <si>
-    <t xml:space="preserve">org.drools.benchmarks.oopath.model.*</t>
+    <t xml:space="preserve">org.drools.benchmarks.model.reactive.*</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -172,6 +178,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -192,6 +199,7 @@
       <sz val="7"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -199,6 +207,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -206,18 +215,21 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="7"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -225,12 +237,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -354,9 +368,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -414,10 +430,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -474,13 +486,13 @@
   <dimension ref="A1:IT111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A112" activeCellId="0" sqref="A112"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="20.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.72"/>
@@ -498,7 +510,7 @@
       <c r="C1" s="3"/>
       <c r="IT1" s="0"/>
     </row>
-    <row r="2" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -511,7 +523,7 @@
       <c r="G2" s="6"/>
       <c r="IT2" s="0"/>
     </row>
-    <row r="3" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -554,7 +566,7 @@
       <c r="IR6" s="0"/>
       <c r="IT6" s="0"/>
     </row>
-    <row r="7" s="15" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="7" s="1" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
@@ -562,7 +574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" s="15" customFormat="true" ht="11.2" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="8" s="1" customFormat="true" ht="11.2" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
@@ -570,835 +582,835 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" s="18" customFormat="true" ht="23.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A9" s="16" t="s">
+    <row r="9" s="17" customFormat="true" ht="23.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>14</v>
       </c>
       <c r="IQ10" s="0"/>
       <c r="IR10" s="0"/>
     </row>
-    <row r="11" s="1" customFormat="true" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="n">
+    <row r="11" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="B11" s="22" t="n">
+      <c r="B11" s="21" t="n">
         <v>10000</v>
       </c>
       <c r="IQ11" s="0"/>
       <c r="IR11" s="0"/>
     </row>
-    <row r="12" s="1" customFormat="true" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="n">
+    <row r="12" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="B12" s="22" t="n">
+      <c r="B12" s="21" t="n">
         <v>10126</v>
       </c>
       <c r="IQ12" s="0"/>
       <c r="IR12" s="0"/>
     </row>
-    <row r="13" s="1" customFormat="true" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="21" t="n">
+    <row r="13" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="B13" s="22" t="n">
+      <c r="B13" s="21" t="n">
         <v>10252</v>
       </c>
       <c r="IQ13" s="0"/>
       <c r="IR13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23" t="n">
+      <c r="A14" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="22" t="n">
+      <c r="B14" s="21" t="n">
         <v>10378</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="n">
+      <c r="A15" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="B15" s="22" t="n">
+      <c r="B15" s="21" t="n">
         <v>10504</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23" t="n">
+      <c r="A16" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="B16" s="22" t="n">
+      <c r="B16" s="21" t="n">
         <v>10630</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="n">
+      <c r="A17" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="B17" s="22" t="n">
+      <c r="B17" s="21" t="n">
         <v>10756</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23" t="n">
+      <c r="A18" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="B18" s="22" t="n">
+      <c r="B18" s="21" t="n">
         <v>10882</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="21" t="n">
+      <c r="A19" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="B19" s="22" t="n">
+      <c r="B19" s="21" t="n">
         <v>11008</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="23" t="n">
+      <c r="A20" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="B20" s="22" t="n">
+      <c r="B20" s="21" t="n">
         <v>11134</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21" t="n">
+      <c r="A21" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="B21" s="22" t="n">
+      <c r="B21" s="21" t="n">
         <v>11260</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="23" t="n">
+      <c r="A22" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="B22" s="22" t="n">
+      <c r="B22" s="21" t="n">
         <v>11386</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21" t="n">
+      <c r="A23" s="20" t="n">
         <v>13</v>
       </c>
-      <c r="B23" s="22" t="n">
+      <c r="B23" s="21" t="n">
         <v>11512</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="23" t="n">
+      <c r="A24" s="22" t="n">
         <v>14</v>
       </c>
-      <c r="B24" s="22" t="n">
+      <c r="B24" s="21" t="n">
         <v>11638</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="21" t="n">
+      <c r="A25" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="B25" s="22" t="n">
+      <c r="B25" s="21" t="n">
         <v>11764</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="23" t="n">
+      <c r="A26" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="B26" s="22" t="n">
+      <c r="B26" s="21" t="n">
         <v>11890</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="21" t="n">
+      <c r="A27" s="20" t="n">
         <v>17</v>
       </c>
-      <c r="B27" s="22" t="n">
+      <c r="B27" s="21" t="n">
         <v>12016</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="23" t="n">
+      <c r="A28" s="22" t="n">
         <v>18</v>
       </c>
-      <c r="B28" s="22" t="n">
+      <c r="B28" s="21" t="n">
         <v>12142</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="21" t="n">
+      <c r="A29" s="20" t="n">
         <v>19</v>
       </c>
-      <c r="B29" s="22" t="n">
+      <c r="B29" s="21" t="n">
         <v>12268</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="23" t="n">
+      <c r="A30" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="B30" s="22" t="n">
+      <c r="B30" s="21" t="n">
         <v>12394</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="21" t="n">
+      <c r="A31" s="20" t="n">
         <v>21</v>
       </c>
-      <c r="B31" s="22" t="n">
+      <c r="B31" s="21" t="n">
         <v>12520</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="23" t="n">
+      <c r="A32" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="B32" s="22" t="n">
+      <c r="B32" s="21" t="n">
         <v>12646</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="21" t="n">
+      <c r="A33" s="20" t="n">
         <v>23</v>
       </c>
-      <c r="B33" s="22" t="n">
+      <c r="B33" s="21" t="n">
         <v>12772</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="23" t="n">
+      <c r="A34" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="B34" s="22" t="n">
+      <c r="B34" s="21" t="n">
         <v>12898</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="21" t="n">
+      <c r="A35" s="20" t="n">
         <v>25</v>
       </c>
-      <c r="B35" s="22" t="n">
+      <c r="B35" s="21" t="n">
         <v>13024</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="23" t="n">
+      <c r="A36" s="22" t="n">
         <v>26</v>
       </c>
-      <c r="B36" s="22" t="n">
+      <c r="B36" s="21" t="n">
         <v>13150</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="21" t="n">
+      <c r="A37" s="20" t="n">
         <v>27</v>
       </c>
-      <c r="B37" s="22" t="n">
+      <c r="B37" s="21" t="n">
         <v>13276</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="23" t="n">
+      <c r="A38" s="22" t="n">
         <v>28</v>
       </c>
-      <c r="B38" s="22" t="n">
+      <c r="B38" s="21" t="n">
         <v>13402</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="21" t="n">
+      <c r="A39" s="20" t="n">
         <v>29</v>
       </c>
-      <c r="B39" s="22" t="n">
+      <c r="B39" s="21" t="n">
         <v>13528</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="23" t="n">
+      <c r="A40" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="B40" s="22" t="n">
+      <c r="B40" s="21" t="n">
         <v>13654</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="23" t="n">
+      <c r="A41" s="22" t="n">
         <v>31</v>
       </c>
-      <c r="B41" s="22" t="n">
+      <c r="B41" s="21" t="n">
         <v>13780</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="23" t="n">
+      <c r="A42" s="22" t="n">
         <v>32</v>
       </c>
-      <c r="B42" s="22" t="n">
+      <c r="B42" s="21" t="n">
         <v>13906</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="23" t="n">
+      <c r="A43" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="B43" s="22" t="n">
+      <c r="B43" s="21" t="n">
         <v>14032</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="23" t="n">
+      <c r="A44" s="22" t="n">
         <v>34</v>
       </c>
-      <c r="B44" s="22" t="n">
+      <c r="B44" s="21" t="n">
         <v>14158</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="23" t="n">
+      <c r="A45" s="22" t="n">
         <v>35</v>
       </c>
-      <c r="B45" s="22" t="n">
+      <c r="B45" s="21" t="n">
         <v>14284</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="23" t="n">
+      <c r="A46" s="22" t="n">
         <v>36</v>
       </c>
-      <c r="B46" s="22" t="n">
+      <c r="B46" s="21" t="n">
         <v>14410</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="23" t="n">
+      <c r="A47" s="22" t="n">
         <v>37</v>
       </c>
-      <c r="B47" s="22" t="n">
+      <c r="B47" s="21" t="n">
         <v>14536</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="23" t="n">
+      <c r="A48" s="22" t="n">
         <v>38</v>
       </c>
-      <c r="B48" s="22" t="n">
+      <c r="B48" s="21" t="n">
         <v>14662</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="23" t="n">
+      <c r="A49" s="22" t="n">
         <v>39</v>
       </c>
-      <c r="B49" s="22" t="n">
+      <c r="B49" s="21" t="n">
         <v>14788</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="23" t="n">
+      <c r="A50" s="22" t="n">
         <v>40</v>
       </c>
-      <c r="B50" s="22" t="n">
+      <c r="B50" s="21" t="n">
         <v>14914</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="23" t="n">
+      <c r="A51" s="22" t="n">
         <v>41</v>
       </c>
-      <c r="B51" s="22" t="n">
+      <c r="B51" s="21" t="n">
         <v>15040</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="23" t="n">
+      <c r="A52" s="22" t="n">
         <v>42</v>
       </c>
-      <c r="B52" s="22" t="n">
+      <c r="B52" s="21" t="n">
         <v>15166</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="23" t="n">
+      <c r="A53" s="22" t="n">
         <v>43</v>
       </c>
-      <c r="B53" s="22" t="n">
+      <c r="B53" s="21" t="n">
         <v>15292</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="23" t="n">
+      <c r="A54" s="22" t="n">
         <v>44</v>
       </c>
-      <c r="B54" s="22" t="n">
+      <c r="B54" s="21" t="n">
         <v>15418</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="23" t="n">
+      <c r="A55" s="22" t="n">
         <v>45</v>
       </c>
-      <c r="B55" s="22" t="n">
+      <c r="B55" s="21" t="n">
         <v>15544</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="23" t="n">
+      <c r="A56" s="22" t="n">
         <v>46</v>
       </c>
-      <c r="B56" s="22" t="n">
+      <c r="B56" s="21" t="n">
         <v>15670</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="23" t="n">
+      <c r="A57" s="22" t="n">
         <v>47</v>
       </c>
-      <c r="B57" s="22" t="n">
+      <c r="B57" s="21" t="n">
         <v>15796</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="23" t="n">
+      <c r="A58" s="22" t="n">
         <v>48</v>
       </c>
-      <c r="B58" s="22" t="n">
+      <c r="B58" s="21" t="n">
         <v>15922</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="23" t="n">
+      <c r="A59" s="22" t="n">
         <v>49</v>
       </c>
-      <c r="B59" s="22" t="n">
+      <c r="B59" s="21" t="n">
         <v>16048</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="23" t="n">
+      <c r="A60" s="22" t="n">
         <v>50</v>
       </c>
-      <c r="B60" s="22" t="n">
+      <c r="B60" s="21" t="n">
         <v>16174</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="23" t="n">
+      <c r="A61" s="22" t="n">
         <v>51</v>
       </c>
-      <c r="B61" s="22" t="n">
+      <c r="B61" s="21" t="n">
         <v>16300</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="23" t="n">
+      <c r="A62" s="22" t="n">
         <v>52</v>
       </c>
-      <c r="B62" s="22" t="n">
+      <c r="B62" s="21" t="n">
         <v>16426</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="23" t="n">
+      <c r="A63" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="B63" s="22" t="n">
+      <c r="B63" s="21" t="n">
         <v>16552</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="23" t="n">
+      <c r="A64" s="22" t="n">
         <v>54</v>
       </c>
-      <c r="B64" s="22" t="n">
+      <c r="B64" s="21" t="n">
         <v>16678</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="23" t="n">
+      <c r="A65" s="22" t="n">
         <v>55</v>
       </c>
-      <c r="B65" s="22" t="n">
+      <c r="B65" s="21" t="n">
         <v>16804</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="23" t="n">
+      <c r="A66" s="22" t="n">
         <v>56</v>
       </c>
-      <c r="B66" s="22" t="n">
+      <c r="B66" s="21" t="n">
         <v>16930</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="23" t="n">
+      <c r="A67" s="22" t="n">
         <v>57</v>
       </c>
-      <c r="B67" s="22" t="n">
+      <c r="B67" s="21" t="n">
         <v>17056</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="23" t="n">
+      <c r="A68" s="22" t="n">
         <v>58</v>
       </c>
-      <c r="B68" s="22" t="n">
+      <c r="B68" s="21" t="n">
         <v>17182</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="23" t="n">
+      <c r="A69" s="22" t="n">
         <v>59</v>
       </c>
-      <c r="B69" s="22" t="n">
+      <c r="B69" s="21" t="n">
         <v>17308</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="23" t="n">
+      <c r="A70" s="22" t="n">
         <v>60</v>
       </c>
-      <c r="B70" s="22" t="n">
+      <c r="B70" s="21" t="n">
         <v>17434</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="23" t="n">
+      <c r="A71" s="22" t="n">
         <v>61</v>
       </c>
-      <c r="B71" s="22" t="n">
+      <c r="B71" s="21" t="n">
         <v>17560</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="23" t="n">
+      <c r="A72" s="22" t="n">
         <v>62</v>
       </c>
-      <c r="B72" s="22" t="n">
+      <c r="B72" s="21" t="n">
         <v>17686</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="23" t="n">
+      <c r="A73" s="22" t="n">
         <v>63</v>
       </c>
-      <c r="B73" s="22" t="n">
+      <c r="B73" s="21" t="n">
         <v>17812</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="23" t="n">
+      <c r="A74" s="22" t="n">
         <v>64</v>
       </c>
-      <c r="B74" s="22" t="n">
+      <c r="B74" s="21" t="n">
         <v>17938</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="23" t="n">
+      <c r="A75" s="22" t="n">
         <v>65</v>
       </c>
-      <c r="B75" s="22" t="n">
+      <c r="B75" s="21" t="n">
         <v>18064</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="23" t="n">
+      <c r="A76" s="22" t="n">
         <v>66</v>
       </c>
-      <c r="B76" s="22" t="n">
+      <c r="B76" s="21" t="n">
         <v>18190</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="23" t="n">
+      <c r="A77" s="22" t="n">
         <v>67</v>
       </c>
-      <c r="B77" s="22" t="n">
+      <c r="B77" s="21" t="n">
         <v>18316</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="23" t="n">
+      <c r="A78" s="22" t="n">
         <v>68</v>
       </c>
-      <c r="B78" s="22" t="n">
+      <c r="B78" s="21" t="n">
         <v>18442</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="23" t="n">
+      <c r="A79" s="22" t="n">
         <v>69</v>
       </c>
-      <c r="B79" s="22" t="n">
+      <c r="B79" s="21" t="n">
         <v>18568</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="23" t="n">
+      <c r="A80" s="22" t="n">
         <v>70</v>
       </c>
-      <c r="B80" s="22" t="n">
+      <c r="B80" s="21" t="n">
         <v>18694</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="23" t="n">
+      <c r="A81" s="22" t="n">
         <v>71</v>
       </c>
-      <c r="B81" s="22" t="n">
+      <c r="B81" s="21" t="n">
         <v>18820</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="23" t="n">
+      <c r="A82" s="22" t="n">
         <v>72</v>
       </c>
-      <c r="B82" s="22" t="n">
+      <c r="B82" s="21" t="n">
         <v>18946</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="23" t="n">
+      <c r="A83" s="22" t="n">
         <v>73</v>
       </c>
-      <c r="B83" s="22" t="n">
+      <c r="B83" s="21" t="n">
         <v>19072</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="23" t="n">
+      <c r="A84" s="22" t="n">
         <v>74</v>
       </c>
-      <c r="B84" s="22" t="n">
+      <c r="B84" s="21" t="n">
         <v>19198</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="23" t="n">
+      <c r="A85" s="22" t="n">
         <v>75</v>
       </c>
-      <c r="B85" s="22" t="n">
+      <c r="B85" s="21" t="n">
         <v>19324</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="23" t="n">
+      <c r="A86" s="22" t="n">
         <v>76</v>
       </c>
-      <c r="B86" s="22" t="n">
+      <c r="B86" s="21" t="n">
         <v>19450</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="23" t="n">
+      <c r="A87" s="22" t="n">
         <v>77</v>
       </c>
-      <c r="B87" s="22" t="n">
+      <c r="B87" s="21" t="n">
         <v>19576</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="23" t="n">
+      <c r="A88" s="22" t="n">
         <v>78</v>
       </c>
-      <c r="B88" s="22" t="n">
+      <c r="B88" s="21" t="n">
         <v>19702</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="23" t="n">
+      <c r="A89" s="22" t="n">
         <v>79</v>
       </c>
-      <c r="B89" s="22" t="n">
+      <c r="B89" s="21" t="n">
         <v>19828</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="23" t="n">
+      <c r="A90" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="B90" s="22" t="n">
+      <c r="B90" s="21" t="n">
         <v>19954</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="23" t="n">
+      <c r="A91" s="22" t="n">
         <v>81</v>
       </c>
-      <c r="B91" s="22" t="n">
+      <c r="B91" s="21" t="n">
         <v>20080</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="23" t="n">
+      <c r="A92" s="22" t="n">
         <v>82</v>
       </c>
-      <c r="B92" s="22" t="n">
+      <c r="B92" s="21" t="n">
         <v>20206</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="23" t="n">
+      <c r="A93" s="22" t="n">
         <v>83</v>
       </c>
-      <c r="B93" s="22" t="n">
+      <c r="B93" s="21" t="n">
         <v>20332</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="23" t="n">
+      <c r="A94" s="22" t="n">
         <v>84</v>
       </c>
-      <c r="B94" s="22" t="n">
+      <c r="B94" s="21" t="n">
         <v>20458</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="23" t="n">
+      <c r="A95" s="22" t="n">
         <v>85</v>
       </c>
-      <c r="B95" s="22" t="n">
+      <c r="B95" s="21" t="n">
         <v>20584</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="23" t="n">
+      <c r="A96" s="22" t="n">
         <v>86</v>
       </c>
-      <c r="B96" s="22" t="n">
+      <c r="B96" s="21" t="n">
         <v>20710</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="23" t="n">
+      <c r="A97" s="22" t="n">
         <v>87</v>
       </c>
-      <c r="B97" s="22" t="n">
+      <c r="B97" s="21" t="n">
         <v>20836</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="23" t="n">
+      <c r="A98" s="22" t="n">
         <v>88</v>
       </c>
-      <c r="B98" s="22" t="n">
+      <c r="B98" s="21" t="n">
         <v>20962</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="23" t="n">
+      <c r="A99" s="22" t="n">
         <v>89</v>
       </c>
-      <c r="B99" s="22" t="n">
+      <c r="B99" s="21" t="n">
         <v>21088</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="23" t="n">
+      <c r="A100" s="22" t="n">
         <v>90</v>
       </c>
-      <c r="B100" s="22" t="n">
+      <c r="B100" s="21" t="n">
         <v>21214</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="23" t="n">
+      <c r="A101" s="22" t="n">
         <v>91</v>
       </c>
-      <c r="B101" s="22" t="n">
+      <c r="B101" s="21" t="n">
         <v>21340</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="23" t="n">
+      <c r="A102" s="22" t="n">
         <v>92</v>
       </c>
-      <c r="B102" s="22" t="n">
+      <c r="B102" s="21" t="n">
         <v>21466</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="23" t="n">
+      <c r="A103" s="22" t="n">
         <v>93</v>
       </c>
-      <c r="B103" s="22" t="n">
+      <c r="B103" s="21" t="n">
         <v>21592</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="23" t="n">
+      <c r="A104" s="22" t="n">
         <v>94</v>
       </c>
-      <c r="B104" s="22" t="n">
+      <c r="B104" s="21" t="n">
         <v>21718</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="23" t="n">
+      <c r="A105" s="22" t="n">
         <v>95</v>
       </c>
-      <c r="B105" s="22" t="n">
+      <c r="B105" s="21" t="n">
         <v>21844</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="23" t="n">
+      <c r="A106" s="22" t="n">
         <v>96</v>
       </c>
-      <c r="B106" s="22" t="n">
+      <c r="B106" s="21" t="n">
         <v>21970</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="23" t="n">
+      <c r="A107" s="22" t="n">
         <v>97</v>
       </c>
-      <c r="B107" s="22" t="n">
+      <c r="B107" s="21" t="n">
         <v>22096</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="23" t="n">
+      <c r="A108" s="22" t="n">
         <v>98</v>
       </c>
-      <c r="B108" s="22" t="n">
+      <c r="B108" s="21" t="n">
         <v>22222</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="23" t="n">
+      <c r="A109" s="22" t="n">
         <v>99</v>
       </c>
-      <c r="B109" s="22" t="n">
+      <c r="B109" s="21" t="n">
         <v>22348</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="23" t="n">
+      <c r="A110" s="22" t="n">
         <v>100</v>
       </c>
-      <c r="B110" s="22" t="n">
+      <c r="B110" s="21" t="n">
         <v>22474</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="23" t="n">
+      <c r="A111" s="22" t="n">
         <v>101</v>
       </c>
-      <c r="B111" s="22" t="n">
+      <c r="B111" s="21" t="n">
         <v>22600</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change OOPath syntax according to [1]
[1] https://issues.jboss.org/browse/DROOLS-1564
</commit_message>
<xml_diff>
--- a/drools-benchmarks/src/main/resources/kbase-creation/oopath-kbase-creation.xlsx
+++ b/drools-benchmarks/src/main/resources/kbase-creation/oopath-kbase-creation.xlsx
@@ -153,7 +153,7 @@
     <t xml:space="preserve">someMan</t>
   </si>
   <si>
-    <t xml:space="preserve">$toy: /wife/children{age &gt; $param}/toys</t>
+    <t xml:space="preserve">$toy: /wife/children[age &gt; $param]/toys</t>
   </si>
   <si>
     <t xml:space="preserve">setAge($param)</t>
@@ -486,7 +486,7 @@
   <dimension ref="A1:IT111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" outlineLevelRow="1" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add OOPath runtime benchmarks (#12)
* Add OOPath runtime benchmarks

* Change OOPath syntax according to [1]

[1] https://issues.jboss.org/browse/DROOLS-1564
</commit_message>
<xml_diff>
--- a/drools-benchmarks/src/main/resources/kbase-creation/oopath-kbase-creation.xlsx
+++ b/drools-benchmarks/src/main/resources/kbase-creation/oopath-kbase-creation.xlsx
@@ -38,6 +38,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">A keyword of "Ruleset" means that this worksheet is a ruleset, and it has a name in the next cell across. In the following lines, we can have imports, or other ruleset directives if we need to ad them in future.
 </t>
@@ -48,6 +49,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Perhaps this is not needed - ruleset name can be XLS name, and imports are not really needed most of the time.</t>
         </r>
@@ -62,6 +64,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Look at me !! I tell you that I am the start of a rule table, and what parameters I require !
 </t>
@@ -72,6 +75,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">(and their types).
 The "RuleTable" keyword must appear on top of the first condition column.
@@ -89,6 +93,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Look at me !!
 </t>
@@ -99,6 +104,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">I tell you that I am a condition colmn. The next row down has the rule "template" and the row below that is a comment. After that, it is all rule data until an empty line !
 Note that if there is no data in a row, then this condition does not apply. 
@@ -123,7 +129,7 @@
     <t xml:space="preserve">Import</t>
   </si>
   <si>
-    <t xml:space="preserve">org.drools.benchmarks.oopath.model.*</t>
+    <t xml:space="preserve">org.drools.benchmarks.model.reactive.*</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -147,7 +153,7 @@
     <t xml:space="preserve">someMan</t>
   </si>
   <si>
-    <t xml:space="preserve">$toy: /wife/children{age &gt; $param}/toys</t>
+    <t xml:space="preserve">$toy: /wife/children[age &gt; $param]/toys</t>
   </si>
   <si>
     <t xml:space="preserve">setAge($param)</t>
@@ -172,6 +178,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -192,6 +199,7 @@
       <sz val="7"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -199,6 +207,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -206,18 +215,21 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="7"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -225,12 +237,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -354,9 +368,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -414,10 +430,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -474,13 +486,13 @@
   <dimension ref="A1:IT111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A112" activeCellId="0" sqref="A112"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="20.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.72"/>
@@ -498,7 +510,7 @@
       <c r="C1" s="3"/>
       <c r="IT1" s="0"/>
     </row>
-    <row r="2" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -511,7 +523,7 @@
       <c r="G2" s="6"/>
       <c r="IT2" s="0"/>
     </row>
-    <row r="3" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -554,7 +566,7 @@
       <c r="IR6" s="0"/>
       <c r="IT6" s="0"/>
     </row>
-    <row r="7" s="15" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="7" s="1" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
@@ -562,7 +574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" s="15" customFormat="true" ht="11.2" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="8" s="1" customFormat="true" ht="11.2" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
@@ -570,835 +582,835 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" s="18" customFormat="true" ht="23.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A9" s="16" t="s">
+    <row r="9" s="17" customFormat="true" ht="23.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>14</v>
       </c>
       <c r="IQ10" s="0"/>
       <c r="IR10" s="0"/>
     </row>
-    <row r="11" s="1" customFormat="true" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="n">
+    <row r="11" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="B11" s="22" t="n">
+      <c r="B11" s="21" t="n">
         <v>10000</v>
       </c>
       <c r="IQ11" s="0"/>
       <c r="IR11" s="0"/>
     </row>
-    <row r="12" s="1" customFormat="true" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="n">
+    <row r="12" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="B12" s="22" t="n">
+      <c r="B12" s="21" t="n">
         <v>10126</v>
       </c>
       <c r="IQ12" s="0"/>
       <c r="IR12" s="0"/>
     </row>
-    <row r="13" s="1" customFormat="true" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="21" t="n">
+    <row r="13" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="B13" s="22" t="n">
+      <c r="B13" s="21" t="n">
         <v>10252</v>
       </c>
       <c r="IQ13" s="0"/>
       <c r="IR13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23" t="n">
+      <c r="A14" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="22" t="n">
+      <c r="B14" s="21" t="n">
         <v>10378</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="n">
+      <c r="A15" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="B15" s="22" t="n">
+      <c r="B15" s="21" t="n">
         <v>10504</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23" t="n">
+      <c r="A16" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="B16" s="22" t="n">
+      <c r="B16" s="21" t="n">
         <v>10630</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="n">
+      <c r="A17" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="B17" s="22" t="n">
+      <c r="B17" s="21" t="n">
         <v>10756</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23" t="n">
+      <c r="A18" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="B18" s="22" t="n">
+      <c r="B18" s="21" t="n">
         <v>10882</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="21" t="n">
+      <c r="A19" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="B19" s="22" t="n">
+      <c r="B19" s="21" t="n">
         <v>11008</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="23" t="n">
+      <c r="A20" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="B20" s="22" t="n">
+      <c r="B20" s="21" t="n">
         <v>11134</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21" t="n">
+      <c r="A21" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="B21" s="22" t="n">
+      <c r="B21" s="21" t="n">
         <v>11260</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="23" t="n">
+      <c r="A22" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="B22" s="22" t="n">
+      <c r="B22" s="21" t="n">
         <v>11386</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21" t="n">
+      <c r="A23" s="20" t="n">
         <v>13</v>
       </c>
-      <c r="B23" s="22" t="n">
+      <c r="B23" s="21" t="n">
         <v>11512</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="23" t="n">
+      <c r="A24" s="22" t="n">
         <v>14</v>
       </c>
-      <c r="B24" s="22" t="n">
+      <c r="B24" s="21" t="n">
         <v>11638</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="21" t="n">
+      <c r="A25" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="B25" s="22" t="n">
+      <c r="B25" s="21" t="n">
         <v>11764</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="23" t="n">
+      <c r="A26" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="B26" s="22" t="n">
+      <c r="B26" s="21" t="n">
         <v>11890</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="21" t="n">
+      <c r="A27" s="20" t="n">
         <v>17</v>
       </c>
-      <c r="B27" s="22" t="n">
+      <c r="B27" s="21" t="n">
         <v>12016</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="23" t="n">
+      <c r="A28" s="22" t="n">
         <v>18</v>
       </c>
-      <c r="B28" s="22" t="n">
+      <c r="B28" s="21" t="n">
         <v>12142</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="21" t="n">
+      <c r="A29" s="20" t="n">
         <v>19</v>
       </c>
-      <c r="B29" s="22" t="n">
+      <c r="B29" s="21" t="n">
         <v>12268</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="23" t="n">
+      <c r="A30" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="B30" s="22" t="n">
+      <c r="B30" s="21" t="n">
         <v>12394</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="21" t="n">
+      <c r="A31" s="20" t="n">
         <v>21</v>
       </c>
-      <c r="B31" s="22" t="n">
+      <c r="B31" s="21" t="n">
         <v>12520</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="23" t="n">
+      <c r="A32" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="B32" s="22" t="n">
+      <c r="B32" s="21" t="n">
         <v>12646</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="21" t="n">
+      <c r="A33" s="20" t="n">
         <v>23</v>
       </c>
-      <c r="B33" s="22" t="n">
+      <c r="B33" s="21" t="n">
         <v>12772</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="23" t="n">
+      <c r="A34" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="B34" s="22" t="n">
+      <c r="B34" s="21" t="n">
         <v>12898</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="21" t="n">
+      <c r="A35" s="20" t="n">
         <v>25</v>
       </c>
-      <c r="B35" s="22" t="n">
+      <c r="B35" s="21" t="n">
         <v>13024</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="23" t="n">
+      <c r="A36" s="22" t="n">
         <v>26</v>
       </c>
-      <c r="B36" s="22" t="n">
+      <c r="B36" s="21" t="n">
         <v>13150</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="21" t="n">
+      <c r="A37" s="20" t="n">
         <v>27</v>
       </c>
-      <c r="B37" s="22" t="n">
+      <c r="B37" s="21" t="n">
         <v>13276</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="23" t="n">
+      <c r="A38" s="22" t="n">
         <v>28</v>
       </c>
-      <c r="B38" s="22" t="n">
+      <c r="B38" s="21" t="n">
         <v>13402</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="21" t="n">
+      <c r="A39" s="20" t="n">
         <v>29</v>
       </c>
-      <c r="B39" s="22" t="n">
+      <c r="B39" s="21" t="n">
         <v>13528</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="23" t="n">
+      <c r="A40" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="B40" s="22" t="n">
+      <c r="B40" s="21" t="n">
         <v>13654</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="23" t="n">
+      <c r="A41" s="22" t="n">
         <v>31</v>
       </c>
-      <c r="B41" s="22" t="n">
+      <c r="B41" s="21" t="n">
         <v>13780</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="23" t="n">
+      <c r="A42" s="22" t="n">
         <v>32</v>
       </c>
-      <c r="B42" s="22" t="n">
+      <c r="B42" s="21" t="n">
         <v>13906</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="23" t="n">
+      <c r="A43" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="B43" s="22" t="n">
+      <c r="B43" s="21" t="n">
         <v>14032</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="23" t="n">
+      <c r="A44" s="22" t="n">
         <v>34</v>
       </c>
-      <c r="B44" s="22" t="n">
+      <c r="B44" s="21" t="n">
         <v>14158</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="23" t="n">
+      <c r="A45" s="22" t="n">
         <v>35</v>
       </c>
-      <c r="B45" s="22" t="n">
+      <c r="B45" s="21" t="n">
         <v>14284</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="23" t="n">
+      <c r="A46" s="22" t="n">
         <v>36</v>
       </c>
-      <c r="B46" s="22" t="n">
+      <c r="B46" s="21" t="n">
         <v>14410</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="23" t="n">
+      <c r="A47" s="22" t="n">
         <v>37</v>
       </c>
-      <c r="B47" s="22" t="n">
+      <c r="B47" s="21" t="n">
         <v>14536</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="23" t="n">
+      <c r="A48" s="22" t="n">
         <v>38</v>
       </c>
-      <c r="B48" s="22" t="n">
+      <c r="B48" s="21" t="n">
         <v>14662</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="23" t="n">
+      <c r="A49" s="22" t="n">
         <v>39</v>
       </c>
-      <c r="B49" s="22" t="n">
+      <c r="B49" s="21" t="n">
         <v>14788</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="23" t="n">
+      <c r="A50" s="22" t="n">
         <v>40</v>
       </c>
-      <c r="B50" s="22" t="n">
+      <c r="B50" s="21" t="n">
         <v>14914</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="23" t="n">
+      <c r="A51" s="22" t="n">
         <v>41</v>
       </c>
-      <c r="B51" s="22" t="n">
+      <c r="B51" s="21" t="n">
         <v>15040</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="23" t="n">
+      <c r="A52" s="22" t="n">
         <v>42</v>
       </c>
-      <c r="B52" s="22" t="n">
+      <c r="B52" s="21" t="n">
         <v>15166</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="23" t="n">
+      <c r="A53" s="22" t="n">
         <v>43</v>
       </c>
-      <c r="B53" s="22" t="n">
+      <c r="B53" s="21" t="n">
         <v>15292</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="23" t="n">
+      <c r="A54" s="22" t="n">
         <v>44</v>
       </c>
-      <c r="B54" s="22" t="n">
+      <c r="B54" s="21" t="n">
         <v>15418</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="23" t="n">
+      <c r="A55" s="22" t="n">
         <v>45</v>
       </c>
-      <c r="B55" s="22" t="n">
+      <c r="B55" s="21" t="n">
         <v>15544</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="23" t="n">
+      <c r="A56" s="22" t="n">
         <v>46</v>
       </c>
-      <c r="B56" s="22" t="n">
+      <c r="B56" s="21" t="n">
         <v>15670</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="23" t="n">
+      <c r="A57" s="22" t="n">
         <v>47</v>
       </c>
-      <c r="B57" s="22" t="n">
+      <c r="B57" s="21" t="n">
         <v>15796</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="23" t="n">
+      <c r="A58" s="22" t="n">
         <v>48</v>
       </c>
-      <c r="B58" s="22" t="n">
+      <c r="B58" s="21" t="n">
         <v>15922</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="23" t="n">
+      <c r="A59" s="22" t="n">
         <v>49</v>
       </c>
-      <c r="B59" s="22" t="n">
+      <c r="B59" s="21" t="n">
         <v>16048</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="23" t="n">
+      <c r="A60" s="22" t="n">
         <v>50</v>
       </c>
-      <c r="B60" s="22" t="n">
+      <c r="B60" s="21" t="n">
         <v>16174</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="23" t="n">
+      <c r="A61" s="22" t="n">
         <v>51</v>
       </c>
-      <c r="B61" s="22" t="n">
+      <c r="B61" s="21" t="n">
         <v>16300</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="23" t="n">
+      <c r="A62" s="22" t="n">
         <v>52</v>
       </c>
-      <c r="B62" s="22" t="n">
+      <c r="B62" s="21" t="n">
         <v>16426</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="23" t="n">
+      <c r="A63" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="B63" s="22" t="n">
+      <c r="B63" s="21" t="n">
         <v>16552</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="23" t="n">
+      <c r="A64" s="22" t="n">
         <v>54</v>
       </c>
-      <c r="B64" s="22" t="n">
+      <c r="B64" s="21" t="n">
         <v>16678</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="23" t="n">
+      <c r="A65" s="22" t="n">
         <v>55</v>
       </c>
-      <c r="B65" s="22" t="n">
+      <c r="B65" s="21" t="n">
         <v>16804</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="23" t="n">
+      <c r="A66" s="22" t="n">
         <v>56</v>
       </c>
-      <c r="B66" s="22" t="n">
+      <c r="B66" s="21" t="n">
         <v>16930</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="23" t="n">
+      <c r="A67" s="22" t="n">
         <v>57</v>
       </c>
-      <c r="B67" s="22" t="n">
+      <c r="B67" s="21" t="n">
         <v>17056</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="23" t="n">
+      <c r="A68" s="22" t="n">
         <v>58</v>
       </c>
-      <c r="B68" s="22" t="n">
+      <c r="B68" s="21" t="n">
         <v>17182</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="23" t="n">
+      <c r="A69" s="22" t="n">
         <v>59</v>
       </c>
-      <c r="B69" s="22" t="n">
+      <c r="B69" s="21" t="n">
         <v>17308</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="23" t="n">
+      <c r="A70" s="22" t="n">
         <v>60</v>
       </c>
-      <c r="B70" s="22" t="n">
+      <c r="B70" s="21" t="n">
         <v>17434</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="23" t="n">
+      <c r="A71" s="22" t="n">
         <v>61</v>
       </c>
-      <c r="B71" s="22" t="n">
+      <c r="B71" s="21" t="n">
         <v>17560</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="23" t="n">
+      <c r="A72" s="22" t="n">
         <v>62</v>
       </c>
-      <c r="B72" s="22" t="n">
+      <c r="B72" s="21" t="n">
         <v>17686</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="23" t="n">
+      <c r="A73" s="22" t="n">
         <v>63</v>
       </c>
-      <c r="B73" s="22" t="n">
+      <c r="B73" s="21" t="n">
         <v>17812</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="23" t="n">
+      <c r="A74" s="22" t="n">
         <v>64</v>
       </c>
-      <c r="B74" s="22" t="n">
+      <c r="B74" s="21" t="n">
         <v>17938</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="23" t="n">
+      <c r="A75" s="22" t="n">
         <v>65</v>
       </c>
-      <c r="B75" s="22" t="n">
+      <c r="B75" s="21" t="n">
         <v>18064</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="23" t="n">
+      <c r="A76" s="22" t="n">
         <v>66</v>
       </c>
-      <c r="B76" s="22" t="n">
+      <c r="B76" s="21" t="n">
         <v>18190</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="23" t="n">
+      <c r="A77" s="22" t="n">
         <v>67</v>
       </c>
-      <c r="B77" s="22" t="n">
+      <c r="B77" s="21" t="n">
         <v>18316</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="23" t="n">
+      <c r="A78" s="22" t="n">
         <v>68</v>
       </c>
-      <c r="B78" s="22" t="n">
+      <c r="B78" s="21" t="n">
         <v>18442</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="23" t="n">
+      <c r="A79" s="22" t="n">
         <v>69</v>
       </c>
-      <c r="B79" s="22" t="n">
+      <c r="B79" s="21" t="n">
         <v>18568</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="23" t="n">
+      <c r="A80" s="22" t="n">
         <v>70</v>
       </c>
-      <c r="B80" s="22" t="n">
+      <c r="B80" s="21" t="n">
         <v>18694</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="23" t="n">
+      <c r="A81" s="22" t="n">
         <v>71</v>
       </c>
-      <c r="B81" s="22" t="n">
+      <c r="B81" s="21" t="n">
         <v>18820</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="23" t="n">
+      <c r="A82" s="22" t="n">
         <v>72</v>
       </c>
-      <c r="B82" s="22" t="n">
+      <c r="B82" s="21" t="n">
         <v>18946</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="23" t="n">
+      <c r="A83" s="22" t="n">
         <v>73</v>
       </c>
-      <c r="B83" s="22" t="n">
+      <c r="B83" s="21" t="n">
         <v>19072</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="23" t="n">
+      <c r="A84" s="22" t="n">
         <v>74</v>
       </c>
-      <c r="B84" s="22" t="n">
+      <c r="B84" s="21" t="n">
         <v>19198</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="23" t="n">
+      <c r="A85" s="22" t="n">
         <v>75</v>
       </c>
-      <c r="B85" s="22" t="n">
+      <c r="B85" s="21" t="n">
         <v>19324</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="23" t="n">
+      <c r="A86" s="22" t="n">
         <v>76</v>
       </c>
-      <c r="B86" s="22" t="n">
+      <c r="B86" s="21" t="n">
         <v>19450</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="23" t="n">
+      <c r="A87" s="22" t="n">
         <v>77</v>
       </c>
-      <c r="B87" s="22" t="n">
+      <c r="B87" s="21" t="n">
         <v>19576</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="23" t="n">
+      <c r="A88" s="22" t="n">
         <v>78</v>
       </c>
-      <c r="B88" s="22" t="n">
+      <c r="B88" s="21" t="n">
         <v>19702</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="23" t="n">
+      <c r="A89" s="22" t="n">
         <v>79</v>
       </c>
-      <c r="B89" s="22" t="n">
+      <c r="B89" s="21" t="n">
         <v>19828</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="23" t="n">
+      <c r="A90" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="B90" s="22" t="n">
+      <c r="B90" s="21" t="n">
         <v>19954</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="23" t="n">
+      <c r="A91" s="22" t="n">
         <v>81</v>
       </c>
-      <c r="B91" s="22" t="n">
+      <c r="B91" s="21" t="n">
         <v>20080</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="23" t="n">
+      <c r="A92" s="22" t="n">
         <v>82</v>
       </c>
-      <c r="B92" s="22" t="n">
+      <c r="B92" s="21" t="n">
         <v>20206</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="23" t="n">
+      <c r="A93" s="22" t="n">
         <v>83</v>
       </c>
-      <c r="B93" s="22" t="n">
+      <c r="B93" s="21" t="n">
         <v>20332</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="23" t="n">
+      <c r="A94" s="22" t="n">
         <v>84</v>
       </c>
-      <c r="B94" s="22" t="n">
+      <c r="B94" s="21" t="n">
         <v>20458</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="23" t="n">
+      <c r="A95" s="22" t="n">
         <v>85</v>
       </c>
-      <c r="B95" s="22" t="n">
+      <c r="B95" s="21" t="n">
         <v>20584</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="23" t="n">
+      <c r="A96" s="22" t="n">
         <v>86</v>
       </c>
-      <c r="B96" s="22" t="n">
+      <c r="B96" s="21" t="n">
         <v>20710</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="23" t="n">
+      <c r="A97" s="22" t="n">
         <v>87</v>
       </c>
-      <c r="B97" s="22" t="n">
+      <c r="B97" s="21" t="n">
         <v>20836</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="23" t="n">
+      <c r="A98" s="22" t="n">
         <v>88</v>
       </c>
-      <c r="B98" s="22" t="n">
+      <c r="B98" s="21" t="n">
         <v>20962</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="23" t="n">
+      <c r="A99" s="22" t="n">
         <v>89</v>
       </c>
-      <c r="B99" s="22" t="n">
+      <c r="B99" s="21" t="n">
         <v>21088</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="23" t="n">
+      <c r="A100" s="22" t="n">
         <v>90</v>
       </c>
-      <c r="B100" s="22" t="n">
+      <c r="B100" s="21" t="n">
         <v>21214</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="23" t="n">
+      <c r="A101" s="22" t="n">
         <v>91</v>
       </c>
-      <c r="B101" s="22" t="n">
+      <c r="B101" s="21" t="n">
         <v>21340</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="23" t="n">
+      <c r="A102" s="22" t="n">
         <v>92</v>
       </c>
-      <c r="B102" s="22" t="n">
+      <c r="B102" s="21" t="n">
         <v>21466</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="23" t="n">
+      <c r="A103" s="22" t="n">
         <v>93</v>
       </c>
-      <c r="B103" s="22" t="n">
+      <c r="B103" s="21" t="n">
         <v>21592</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="23" t="n">
+      <c r="A104" s="22" t="n">
         <v>94</v>
       </c>
-      <c r="B104" s="22" t="n">
+      <c r="B104" s="21" t="n">
         <v>21718</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="23" t="n">
+      <c r="A105" s="22" t="n">
         <v>95</v>
       </c>
-      <c r="B105" s="22" t="n">
+      <c r="B105" s="21" t="n">
         <v>21844</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="23" t="n">
+      <c r="A106" s="22" t="n">
         <v>96</v>
       </c>
-      <c r="B106" s="22" t="n">
+      <c r="B106" s="21" t="n">
         <v>21970</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="23" t="n">
+      <c r="A107" s="22" t="n">
         <v>97</v>
       </c>
-      <c r="B107" s="22" t="n">
+      <c r="B107" s="21" t="n">
         <v>22096</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="23" t="n">
+      <c r="A108" s="22" t="n">
         <v>98</v>
       </c>
-      <c r="B108" s="22" t="n">
+      <c r="B108" s="21" t="n">
         <v>22222</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="23" t="n">
+      <c r="A109" s="22" t="n">
         <v>99</v>
       </c>
-      <c r="B109" s="22" t="n">
+      <c r="B109" s="21" t="n">
         <v>22348</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="23" t="n">
+      <c r="A110" s="22" t="n">
         <v>100</v>
       </c>
-      <c r="B110" s="22" t="n">
+      <c r="B110" s="21" t="n">
         <v>22474</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="23" t="n">
+      <c r="A111" s="22" t="n">
         <v>101</v>
       </c>
-      <c r="B111" s="22" t="n">
+      <c r="B111" s="21" t="n">
         <v>22600</v>
       </c>
     </row>

</xml_diff>